<commit_message>
make the battle scene can enter
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/MainIcon.xlsx
+++ b/ConfigData/Xlsx/MainIcon.xlsx
@@ -86,25 +86,13 @@
     <t>打开主菜单(ESC)</t>
   </si>
   <si>
-    <t>MainIcon1</t>
-  </si>
-  <si>
     <t>商城</t>
   </si>
   <si>
-    <t>MainIcon8</t>
-  </si>
-  <si>
     <t>挑战</t>
   </si>
   <si>
-    <t>MainIcon5</t>
-  </si>
-  <si>
     <t>物品</t>
-  </si>
-  <si>
-    <t>MainIcon2</t>
   </si>
   <si>
     <t>int</t>
@@ -163,10 +151,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>SideButton4</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>序列</t>
   </si>
   <si>
@@ -231,10 +215,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>MainIcon3</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>查看我的物品</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -259,7 +239,26 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>MainIcon10</t>
+    <t>mainicon1</t>
+  </si>
+  <si>
+    <t>mainicon8</t>
+  </si>
+  <si>
+    <t>mainicon3</t>
+  </si>
+  <si>
+    <t>mainicon5</t>
+  </si>
+  <si>
+    <t>mainicon2</t>
+  </si>
+  <si>
+    <t>mainicon10</t>
+  </si>
+  <si>
+    <t>sidebutton4</t>
+    <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1410,7 +1409,7 @@
   <dimension ref="A1:N10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1426,134 +1425,134 @@
   <sheetData>
     <row r="1" spans="1:14" ht="57" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="G1" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="I1" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="M1" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="G1" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="I1" s="4" t="s">
+      <c r="N1" s="4" t="s">
         <v>32</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="N1" s="4" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="G3" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="I3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="J3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="K3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="L3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G3" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="I3" s="2" t="s">
+      <c r="M3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="N3" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M3" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="N3" s="2" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.15">
@@ -1573,10 +1572,10 @@
         <v>0</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="I4">
         <v>-82</v>
@@ -1594,7 +1593,7 @@
         <v>0</v>
       </c>
       <c r="N4" t="s">
-        <v>1</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.15">
@@ -1602,10 +1601,10 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -1617,10 +1616,10 @@
         <v>10</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="I5">
         <v>0</v>
@@ -1638,7 +1637,7 @@
         <v>1</v>
       </c>
       <c r="N5" t="s">
-        <v>3</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.15">
@@ -1646,10 +1645,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C6" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -1661,10 +1660,10 @@
         <v>0</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="I6">
         <v>0</v>
@@ -1682,7 +1681,7 @@
         <v>1</v>
       </c>
       <c r="N6" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.15">
@@ -1690,10 +1689,10 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -1705,10 +1704,10 @@
         <v>4</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="I7">
         <v>0</v>
@@ -1726,7 +1725,7 @@
         <v>1</v>
       </c>
       <c r="N7" t="s">
-        <v>5</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.15">
@@ -1734,10 +1733,10 @@
         <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C8" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -1749,10 +1748,10 @@
         <v>0</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="I8">
         <v>0</v>
@@ -1770,7 +1769,7 @@
         <v>1</v>
       </c>
       <c r="N8" t="s">
-        <v>7</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.15">
@@ -1778,10 +1777,10 @@
         <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="C9" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="D9">
         <v>0</v>
@@ -1793,10 +1792,10 @@
         <v>0</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="I9">
         <v>0</v>
@@ -1814,7 +1813,7 @@
         <v>1</v>
       </c>
       <c r="N9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.15">
@@ -1822,10 +1821,10 @@
         <v>42</v>
       </c>
       <c r="B10" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C10" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D10">
         <v>0</v>
@@ -1837,10 +1836,10 @@
         <v>50</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="I10">
         <v>0</v>
@@ -1858,7 +1857,7 @@
         <v>2</v>
       </c>
       <c r="N10" t="s">
-        <v>25</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>